<commit_message>
excel util updated and log4j example added
</commit_message>
<xml_diff>
--- a/Vytracktestdata.xlsx
+++ b/Vytracktestdata.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3842" uniqueCount="1476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3849" uniqueCount="1476">
   <si>
     <t>username</t>
   </si>
@@ -4824,8 +4824,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.6640625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.83203125"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -9068,8 +9068,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.6640625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.83203125"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -9360,7 +9360,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.83203125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -13607,7 +13607,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.83203125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -13898,7 +13898,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.83203125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -18145,7 +18145,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.83203125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>